<commit_message>
FCT og ICR data behandling
</commit_message>
<xml_diff>
--- a/data/FCT/FCT_samlet.xlsx
+++ b/data/FCT/FCT_samlet.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://grundfos-my.sharepoint.com/personal/102222_grundfos_com/Documents/Desktop/Speciale/data/FCT/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="18" documentId="8_{1BAE84E1-28FB-4C31-9EA8-35FF7732D87F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0D797C4D-F308-4402-A92C-DFE9539BEEB1}"/>
+  <xr:revisionPtr revIDLastSave="65" documentId="8_{1BAE84E1-28FB-4C31-9EA8-35FF7732D87F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{301C513B-4FA1-40E6-A437-0C2014DF4C74}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{926BA01D-7E05-4040-85F6-3A23D61AC3DF}"/>
+    <workbookView xWindow="2955" yWindow="1095" windowWidth="21600" windowHeight="11385" activeTab="4" xr2:uid="{926BA01D-7E05-4040-85F6-3A23D61AC3DF}"/>
   </bookViews>
   <sheets>
     <sheet name="FCT 1A " sheetId="2" r:id="rId1"/>
     <sheet name="FCT 1B" sheetId="1" r:id="rId2"/>
     <sheet name="FCT 2A " sheetId="3" r:id="rId3"/>
     <sheet name="FCT 2B" sheetId="4" r:id="rId4"/>
+    <sheet name="Dunk" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="30">
   <si>
     <t>name</t>
   </si>
@@ -91,6 +92,42 @@
   </si>
   <si>
     <t>FCT_2B</t>
+  </si>
+  <si>
+    <t>D1</t>
+  </si>
+  <si>
+    <t>D2</t>
+  </si>
+  <si>
+    <t>D3</t>
+  </si>
+  <si>
+    <t>D4</t>
+  </si>
+  <si>
+    <t>FCT_1A SiO2</t>
+  </si>
+  <si>
+    <t>FCT_1B SiO2</t>
+  </si>
+  <si>
+    <t>FCT_2A SiO2</t>
+  </si>
+  <si>
+    <t>FCT_2B SiO2</t>
+  </si>
+  <si>
+    <t>FCT_1A Cl</t>
+  </si>
+  <si>
+    <t>FCT_1BCl</t>
+  </si>
+  <si>
+    <t>FCT_2A Cl</t>
+  </si>
+  <si>
+    <t>FCT_2B Cl</t>
   </si>
 </sst>
 </file>
@@ -445,7 +482,7 @@
   <dimension ref="A1:N6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection sqref="A1:N6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -902,8 +939,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B4DB096-B3FC-4198-AE8E-095264C93D54}">
   <dimension ref="A1:N6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J3" sqref="J3:J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -964,6 +1001,12 @@
       <c r="B2">
         <v>0</v>
       </c>
+      <c r="C2">
+        <v>42.6</v>
+      </c>
+      <c r="D2">
+        <v>56.2</v>
+      </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -972,6 +1015,18 @@
       <c r="B3">
         <v>1.5</v>
       </c>
+      <c r="C3">
+        <v>41.6</v>
+      </c>
+      <c r="D3">
+        <v>56.4</v>
+      </c>
+      <c r="I3">
+        <v>35</v>
+      </c>
+      <c r="J3">
+        <v>60</v>
+      </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -980,6 +1035,18 @@
       <c r="B4">
         <v>4</v>
       </c>
+      <c r="C4">
+        <v>43.8</v>
+      </c>
+      <c r="D4">
+        <v>53</v>
+      </c>
+      <c r="I4">
+        <v>37.4</v>
+      </c>
+      <c r="J4">
+        <v>61</v>
+      </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
@@ -988,6 +1055,18 @@
       <c r="B5">
         <v>6.5</v>
       </c>
+      <c r="C5">
+        <v>46.4</v>
+      </c>
+      <c r="D5">
+        <v>49.4</v>
+      </c>
+      <c r="I5">
+        <v>39.6</v>
+      </c>
+      <c r="J5">
+        <v>62.6</v>
+      </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
@@ -995,10 +1074,174 @@
       </c>
       <c r="B6">
         <v>7.25</v>
+      </c>
+      <c r="C6">
+        <v>48.2</v>
+      </c>
+      <c r="D6">
+        <v>49.8</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42EB39FE-0B87-4D76-B4D3-FA229DA848B6}">
+  <dimension ref="A1:J5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L10" sqref="L10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="11.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G1" t="s">
+        <v>26</v>
+      </c>
+      <c r="H1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I1" t="s">
+        <v>28</v>
+      </c>
+      <c r="J1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2">
+        <f>2100/1002</f>
+        <v>2.0958083832335328</v>
+      </c>
+      <c r="C2">
+        <v>41.4</v>
+      </c>
+      <c r="D2">
+        <v>38.4</v>
+      </c>
+      <c r="E2">
+        <v>37.200000000000003</v>
+      </c>
+      <c r="F2">
+        <v>35.1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3">
+        <f>4200/1002</f>
+        <v>4.1916167664670656</v>
+      </c>
+      <c r="C3">
+        <v>43</v>
+      </c>
+      <c r="D3">
+        <v>40.299999999999997</v>
+      </c>
+      <c r="E3">
+        <v>39.5</v>
+      </c>
+      <c r="F3">
+        <v>35.6</v>
+      </c>
+      <c r="G3">
+        <v>87.4</v>
+      </c>
+      <c r="H3">
+        <v>81.400000000000006</v>
+      </c>
+      <c r="I3">
+        <v>71.400000000000006</v>
+      </c>
+      <c r="J3">
+        <v>59.2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4">
+        <f>3600/1002</f>
+        <v>3.5928143712574849</v>
+      </c>
+      <c r="C4">
+        <v>47.2</v>
+      </c>
+      <c r="D4">
+        <v>41.3</v>
+      </c>
+      <c r="E4">
+        <v>41.3</v>
+      </c>
+      <c r="F4">
+        <v>36.700000000000003</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5">
+        <f>8800/1002</f>
+        <v>8.7824351297405183</v>
+      </c>
+      <c r="C5">
+        <v>49.6</v>
+      </c>
+      <c r="D5">
+        <v>46.5</v>
+      </c>
+      <c r="E5">
+        <v>46.3</v>
+      </c>
+      <c r="F5">
+        <v>38.299999999999997</v>
+      </c>
+      <c r="G5">
+        <v>72.2</v>
+      </c>
+      <c r="H5">
+        <v>87.4</v>
+      </c>
+      <c r="I5">
+        <v>61.2</v>
+      </c>
+      <c r="J5">
+        <v>69.8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>